<commit_message>
clean docs and interface
</commit_message>
<xml_diff>
--- a/templates/Report_Template.xlsx
+++ b/templates/Report_Template.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cymat-my.sharepoint.com/personal/jjames_cymat_com/Documents/Documents/Python Scripts/Engineering_concepts/SS_Decople/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="117" documentId="8_{4FB79548-BDE1-408D-A523-A3BD55B6D081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B4209E6-9D02-4B69-9FC4-35322718AE5A}"/>
+  <xr:revisionPtr revIDLastSave="182" documentId="8_{4FB79548-BDE1-408D-A523-A3BD55B6D081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B803D90B-37A1-43D4-B119-9EAE599EDE69}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{C420AECD-758F-4CF1-941A-42473DF8134C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C420AECD-758F-4CF1-941A-42473DF8134C}"/>
   </bookViews>
   <sheets>
     <sheet name="1.Summary" sheetId="3" r:id="rId1"/>
     <sheet name="2.Raw_Data" sheetId="2" r:id="rId2"/>
     <sheet name="3.Calculated_Data" sheetId="4" r:id="rId3"/>
-    <sheet name="5.Graphs&amp;Plots" sheetId="5" r:id="rId4"/>
-    <sheet name="6.Test_Procedure" sheetId="6" r:id="rId5"/>
-    <sheet name="7.Statistical_Analysis" sheetId="7" r:id="rId6"/>
+    <sheet name="7.Statistical_Analysis" sheetId="7" r:id="rId4"/>
+    <sheet name="5.Graphs&amp;Plots" sheetId="5" r:id="rId5"/>
+    <sheet name="6.Test_Procedure" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="Analyzed_by">'1.Summary'!$D$12</definedName>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">Material </t>
   </si>
@@ -74,9 +74,6 @@
     <t>Report Date</t>
   </si>
   <si>
-    <t>Project Title</t>
-  </si>
-  <si>
     <t>Company Logo</t>
   </si>
   <si>
@@ -119,9 +116,6 @@
     <t>Energy Absorbtivity [Densifcation]</t>
   </si>
   <si>
-    <t>Plot</t>
-  </si>
-  <si>
     <t>Sample_Title</t>
   </si>
   <si>
@@ -129,18 +123,50 @@
   </si>
   <si>
     <t>Test to ensure conformance with X</t>
+  </si>
+  <si>
+    <t>Example_Group</t>
+  </si>
+  <si>
+    <t>S1, S2, S4, S7</t>
+  </si>
+  <si>
+    <t>MetaData</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Project Title:</t>
+  </si>
+  <si>
+    <t>Graph</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -182,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -197,16 +223,170 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="17">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical style="dashed">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="dashed">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Metadata_Summary_Table" pivot="0" count="4" xr9:uid="{EC4DCA23-3FB1-4B6F-BE73-1F879893CCCE}">
+      <tableStyleElement type="wholeTable" dxfId="13"/>
+      <tableStyleElement type="headerRow" dxfId="11"/>
+      <tableStyleElement type="lastColumn" dxfId="12"/>
+    </tableStyle>
+    <tableStyle name="Overview_Table" pivot="0" count="4" xr9:uid="{436F2976-3570-47D9-B02F-DCEEFCA0E2BE}">
+      <tableStyleElement type="wholeTable" dxfId="10"/>
+      <tableStyleElement type="headerRow" dxfId="9"/>
+      <tableStyleElement type="firstRowStripe" dxfId="8"/>
+      <tableStyleElement type="secondRowStripe" dxfId="7"/>
+    </tableStyle>
+  </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="FF1E8BBC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -216,6 +396,42 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4ECE659C-97FF-4DEB-B157-DFA1DC499CEE}" name="Metadata_Summary_Table" displayName="Metadata_Summary_Table" ref="C6:D13" totalsRowShown="0" headerRowDxfId="16">
+  <autoFilter ref="C6:D13" xr:uid="{4ECE659C-97FF-4DEB-B157-DFA1DC499CEE}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{F8B8869B-3A31-4986-BEE9-A0D6ACE39877}" name="MetaData" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{7A1CCD95-2B8F-4FB2-A167-278F1DF907A9}" name="Value" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="Metadata_Summary_Table" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B4483AC3-E25B-45F6-85DC-9CDE8C758EC6}" name="Table2" displayName="Table2" ref="F3:K4" totalsRowShown="0" dataDxfId="0">
+  <autoFilter ref="F3:K4" xr:uid="{B4483AC3-E25B-45F6-85DC-9CDE8C758EC6}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{74FF3316-F6B9-401C-9588-864A569B52F9}" name="Collective_Name" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{33E84A3F-ACB8-44F5-A0E1-F02C26D1D39B}" name="Samples" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{B64C98CC-6083-4F85-AC3E-DC798B123F1E}" name="Yield_Strength" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{A0A801AB-5758-4F3E-9EFB-A2E390C6F6D2}" name="Maximun Compressive Strength" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{4AB6DA85-6E87-4F91-A989-AACCAA6ADBE1}" name="Young Modules" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{F5B85ED6-0077-4F20-BB3A-E1E12E86E8E3}" name="Energy Absorbtivity [Densifcation]" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="Overview_Table" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -537,65 +753,94 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE034467-D928-4D01-B8AD-52D670698238}">
   <dimension ref="B2:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="29.109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.77734375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="1"/>
-    <col min="7" max="11" width="13.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="14.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="27.88671875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="29.33203125" style="1" customWidth="1"/>
     <col min="12" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="2:11" ht="21" x14ac:dyDescent="0.4">
+      <c r="B2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="C3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="K3" s="11" t="s">
         <v>18</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>45463</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="12">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="I4" s="12">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="J4" s="12">
+        <v>22.36</v>
+      </c>
+      <c r="K4" s="12">
+        <v>432.26</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
@@ -603,7 +848,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.3">
@@ -611,12 +856,12 @@
         <v>3</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" s="5">
         <v>44463</v>
@@ -624,7 +869,7 @@
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
@@ -640,10 +885,10 @@
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C12" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
@@ -651,16 +896,20 @@
         <v>1</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="F14" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="F14" s="13" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -686,6 +935,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E5A8315-CA09-4C6A-9DED-12D56EF24D36}">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FA3A95C-B8BF-4B5C-BF2F-3C1EE9476EFB}">
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -698,11 +965,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DD87ED5-20C3-4163-BE49-811D691BD5A4}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -714,7 +983,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9427D45A-1187-4551-8529-A46CA0358CF3}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -728,20 +997,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FA3A95C-B8BF-4B5C-BF2F-3C1EE9476EFB}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="4" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.88671875" style="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>